<commit_message>
fastapi endpoints with data pipeline in progress
</commit_message>
<xml_diff>
--- a/data/processed/documents/APP-000002/assets_liabilities.xlsx
+++ b/data/processed/documents/APP-000002/assets_liabilities.xlsx
@@ -502,7 +502,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tariq Al Bloushi</t>
+          <t>Kamal Al Shehhi</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5500</v>
+        <v>2480.82</v>
       </c>
     </row>
     <row r="6">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>40483</v>
+        <v>4833</v>
       </c>
     </row>
     <row r="7">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>42578</v>
+        <v>9516</v>
       </c>
     </row>
     <row r="8">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>-2095</v>
+        <v>-4683</v>
       </c>
     </row>
     <row r="9">
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>0.95</v>
+        <v>0.51</v>
       </c>
     </row>
   </sheetData>
@@ -570,7 +570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,41 +603,26 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Vehicles</t>
+          <t>Liquid Assets</t>
         </is>
       </c>
       <c r="B2" s="7" t="inlineStr">
         <is>
-          <t>Economy Car</t>
+          <t>Savings Account</t>
         </is>
       </c>
       <c r="C2" s="8" t="n">
-        <v>34197</v>
+        <v>4833</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
-        <is>
-          <t>Liquid Assets</t>
-        </is>
-      </c>
-      <c r="B3" s="7" t="inlineStr">
-        <is>
-          <t>Savings Account</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="n">
-        <v>6286</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>TOTAL ASSETS</t>
         </is>
       </c>
-      <c r="C4" s="10" t="n">
-        <v>40483</v>
+      <c r="C3" s="10" t="n">
+        <v>4833</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,53 +681,32 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Auto Loans</t>
+          <t>Credit Cards</t>
         </is>
       </c>
       <c r="B2" s="7" t="inlineStr">
         <is>
-          <t>Vehicle Loan 1</t>
+          <t>Credit Card Balance</t>
         </is>
       </c>
       <c r="C2" s="8" t="n">
-        <v>20518</v>
+        <v>9516</v>
       </c>
       <c r="D2" s="8" t="n">
-        <v>427</v>
+        <v>476</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
-        <is>
-          <t>Credit Cards</t>
-        </is>
-      </c>
-      <c r="B3" s="7" t="inlineStr">
-        <is>
-          <t>Credit Card Balance</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="n">
-        <v>22060</v>
-      </c>
-      <c r="D3" s="8" t="n">
-        <v>1103</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>TOTAL LIABILITIES</t>
         </is>
       </c>
-      <c r="C4" s="12" t="n">
-        <v>42578</v>
+      <c r="C3" s="12" t="n">
+        <v>9516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>